<commit_message>
full user story list
all user stories together
</commit_message>
<xml_diff>
--- a/User_Stories/Software_Engineering_UserStories!!!.xlsx
+++ b/User_Stories/Software_Engineering_UserStories!!!.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin mills\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin mills\Desktop\Year3_SoftwareEngineering3_Assignment\User_Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA2758-8D6C-48C2-B8CD-97B92A792C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9571A316-28AD-41F3-AEAC-F8D2A59C3A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{70964867-2F06-4169-9D31-570737C9BC64}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{70964867-2F06-4169-9D31-570737C9BC64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t>Daily Delivery List for Delivery Person</t>
   </si>
@@ -365,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +425,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -481,7 +487,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,13 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,6 +514,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -853,132 +879,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40D65BC-CAAB-4413-8269-BC3843477A14}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="51.7109375" customWidth="1"/>
     <col min="3" max="3" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="18">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="18">
         <v>4</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1123,95 +1149,100 @@
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="18">
         <v>8</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="19" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
+      <c r="A38" s="20">
         <v>9</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="21"/>
+      <c r="B41" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -1409,151 +1440,337 @@
       <c r="C69" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="13">
+      <c r="A73" s="10">
         <v>1</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="14" t="s">
+      <c r="A74" s="10"/>
+      <c r="B74" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="14" t="s">
+      <c r="A75" s="10"/>
+      <c r="B75" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C75" s="12"/>
+      <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="13">
+      <c r="A77" s="10">
         <v>2</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="14" t="s">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C78" s="12"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="14" t="s">
+      <c r="A79" s="10"/>
+      <c r="B79" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C79" s="12"/>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="14" t="s">
+      <c r="A80" s="10"/>
+      <c r="B80" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C80" s="12"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
+      <c r="A82" s="10">
         <v>3</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="14" t="s">
+      <c r="A83" s="10"/>
+      <c r="B83" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="11" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="14" t="s">
+      <c r="A84" s="10"/>
+      <c r="B84" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+      <c r="A86" s="10">
         <v>4</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
-      <c r="B87" s="14" t="s">
+      <c r="A87" s="10"/>
+      <c r="B87" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
-      <c r="B88" s="14" t="s">
+      <c r="A88" s="10"/>
+      <c r="B88" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C88" s="11" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="4">
+        <v>8</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94" s="5"/>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4">
+        <v>2</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="5"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>5</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="4">
+        <v>7</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="13">
+        <v>9</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="14"/>
+      <c r="B109" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="14"/>
+      <c r="B110" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="14"/>
+      <c r="B111" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="14"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>